<commit_message>
Dinosaur initial balancing completed, also rotated all models so that they dont slide sideways
</commit_message>
<xml_diff>
--- a/Balancing research/Dinosaur balancing sheet (OC).xlsx
+++ b/Balancing research/Dinosaur balancing sheet (OC).xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\level-6-l6-group-4\Art Assets\Research\Balancing research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\level-6-l6-group-4\Balancing research\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="86">
   <si>
     <t>Large Carnivore</t>
   </si>
@@ -288,6 +288,12 @@
   </si>
   <si>
     <t>Speed also accounts the amount and weight of a material on the dinosaur, and whether the design would impede movement</t>
+  </si>
+  <si>
+    <t>All variables other than speed and max hp for now are not based on research for the sake of speed</t>
+  </si>
+  <si>
+    <t>Combat range was discerned using the size of the model itself</t>
   </si>
 </sst>
 </file>
@@ -365,9 +371,6 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -377,6 +380,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -694,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3D1E229-3B55-4949-A4CC-FF7D0DB825C8}">
   <dimension ref="A1:AB77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10:M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,15 +713,15 @@
     <col min="25" max="25" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>12</v>
       </c>
       <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
       </c>
       <c r="F1" t="s">
         <v>14</v>
@@ -727,12 +733,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -740,10 +746,10 @@
         <v>7.1</v>
       </c>
       <c r="D3">
+        <v>6.5</v>
+      </c>
+      <c r="E3">
         <v>6.8</v>
-      </c>
-      <c r="E3">
-        <v>6.5</v>
       </c>
       <c r="F3">
         <v>6.7</v>
@@ -755,7 +761,7 @@
         <v>6.45</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -763,10 +769,10 @@
         <v>65</v>
       </c>
       <c r="D4">
+        <v>78</v>
+      </c>
+      <c r="E4">
         <v>85</v>
-      </c>
-      <c r="E4">
-        <v>78</v>
       </c>
       <c r="F4">
         <v>101</v>
@@ -775,40 +781,136 @@
         <v>120</v>
       </c>
       <c r="H4">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="N4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <v>15</v>
+      </c>
+      <c r="G5">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>15</v>
+      </c>
+      <c r="N5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>65</v>
+      </c>
+      <c r="D6">
+        <v>65</v>
+      </c>
+      <c r="E6">
+        <v>65</v>
+      </c>
+      <c r="F6">
+        <v>65</v>
+      </c>
+      <c r="G6">
+        <v>65</v>
+      </c>
+      <c r="H6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>25</v>
+      </c>
+      <c r="D7">
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <v>35</v>
+      </c>
+      <c r="F7">
+        <v>35</v>
+      </c>
+      <c r="G7">
+        <v>35</v>
+      </c>
+      <c r="H7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>4.5</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>180</v>
+      </c>
+      <c r="D9">
+        <v>180</v>
+      </c>
+      <c r="E9">
+        <v>180</v>
+      </c>
+      <c r="F9">
+        <v>180</v>
+      </c>
+      <c r="G9">
+        <v>180</v>
+      </c>
+      <c r="H9">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -816,10 +918,10 @@
         <v>8.85</v>
       </c>
       <c r="D11">
+        <v>8.6</v>
+      </c>
+      <c r="E11">
         <v>8.5500000000000007</v>
-      </c>
-      <c r="E11">
-        <v>8.6</v>
       </c>
       <c r="F11">
         <v>8.3000000000000007</v>
@@ -831,7 +933,7 @@
         <v>8.35</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>1</v>
       </c>
@@ -839,10 +941,10 @@
         <v>35</v>
       </c>
       <c r="D12">
+        <v>47</v>
+      </c>
+      <c r="E12">
         <v>50</v>
-      </c>
-      <c r="E12">
-        <v>47</v>
       </c>
       <c r="F12">
         <v>50</v>
@@ -851,33 +953,123 @@
         <v>65</v>
       </c>
       <c r="H12">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+      <c r="H13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>40</v>
+      </c>
+      <c r="D14">
+        <v>40</v>
+      </c>
+      <c r="E14">
+        <v>40</v>
+      </c>
+      <c r="F14">
+        <v>40</v>
+      </c>
+      <c r="G14">
+        <v>40</v>
+      </c>
+      <c r="H14">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>15</v>
+      </c>
+      <c r="F15">
+        <v>20</v>
+      </c>
+      <c r="G15">
+        <v>25</v>
+      </c>
+      <c r="H15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>5</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>3.5</v>
+      </c>
+      <c r="G16">
+        <v>3.5</v>
+      </c>
+      <c r="H16">
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>6</v>
       </c>
+      <c r="C17">
+        <v>180</v>
+      </c>
+      <c r="D17">
+        <v>180</v>
+      </c>
+      <c r="E17">
+        <v>180</v>
+      </c>
+      <c r="F17">
+        <v>180</v>
+      </c>
+      <c r="G17">
+        <v>180</v>
+      </c>
+      <c r="H17">
+        <v>180</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -892,10 +1084,10 @@
         <v>5.9</v>
       </c>
       <c r="D19">
+        <v>5.35</v>
+      </c>
+      <c r="E19">
         <v>5.4</v>
-      </c>
-      <c r="E19">
-        <v>5.35</v>
       </c>
       <c r="F19">
         <v>5</v>
@@ -915,10 +1107,10 @@
         <v>100</v>
       </c>
       <c r="D20">
+        <v>130</v>
+      </c>
+      <c r="E20">
         <v>135</v>
-      </c>
-      <c r="E20">
-        <v>130</v>
       </c>
       <c r="F20">
         <v>175</v>
@@ -927,33 +1119,123 @@
         <v>160</v>
       </c>
       <c r="H20">
-        <v>190</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>2</v>
       </c>
+      <c r="C21">
+        <v>10</v>
+      </c>
+      <c r="D21">
+        <v>10</v>
+      </c>
+      <c r="E21">
+        <v>10</v>
+      </c>
+      <c r="F21">
+        <v>10</v>
+      </c>
+      <c r="G21">
+        <v>10</v>
+      </c>
+      <c r="H21">
+        <v>10</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>3</v>
       </c>
+      <c r="C22">
+        <v>100</v>
+      </c>
+      <c r="D22">
+        <v>100</v>
+      </c>
+      <c r="E22">
+        <v>100</v>
+      </c>
+      <c r="F22">
+        <v>100</v>
+      </c>
+      <c r="G22">
+        <v>100</v>
+      </c>
+      <c r="H22">
+        <v>100</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>4</v>
       </c>
+      <c r="C23">
+        <v>20</v>
+      </c>
+      <c r="D23">
+        <v>20</v>
+      </c>
+      <c r="E23">
+        <v>25</v>
+      </c>
+      <c r="F23">
+        <v>35</v>
+      </c>
+      <c r="G23">
+        <v>30</v>
+      </c>
+      <c r="H23">
+        <v>40</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>5</v>
       </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
+      </c>
+      <c r="F24">
+        <v>7</v>
+      </c>
+      <c r="G24">
+        <v>6</v>
+      </c>
+      <c r="H24">
+        <v>7</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>6</v>
       </c>
+      <c r="C25">
+        <v>300</v>
+      </c>
+      <c r="D25">
+        <v>300</v>
+      </c>
+      <c r="E25">
+        <v>300</v>
+      </c>
+      <c r="F25">
+        <v>300</v>
+      </c>
+      <c r="G25">
+        <v>300</v>
+      </c>
+      <c r="H25">
+        <v>300</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -968,10 +1250,10 @@
         <v>8.25</v>
       </c>
       <c r="D27">
+        <v>7.9</v>
+      </c>
+      <c r="E27">
         <v>8.1</v>
-      </c>
-      <c r="E27">
-        <v>7.9</v>
       </c>
       <c r="F27">
         <v>7</v>
@@ -991,10 +1273,10 @@
         <v>35</v>
       </c>
       <c r="D28">
+        <v>39</v>
+      </c>
+      <c r="E28">
         <v>45</v>
-      </c>
-      <c r="E28">
-        <v>39</v>
       </c>
       <c r="F28">
         <v>56</v>
@@ -1003,57 +1285,147 @@
         <v>49</v>
       </c>
       <c r="H28">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>2</v>
       </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
+      <c r="F29">
+        <v>4</v>
+      </c>
+      <c r="G29">
+        <v>4</v>
+      </c>
+      <c r="H29">
+        <v>4</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>3</v>
       </c>
+      <c r="C30">
+        <v>30</v>
+      </c>
+      <c r="D30">
+        <v>30</v>
+      </c>
+      <c r="E30">
+        <v>30</v>
+      </c>
+      <c r="F30">
+        <v>30</v>
+      </c>
+      <c r="G30">
+        <v>30</v>
+      </c>
+      <c r="H30">
+        <v>30</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>4</v>
       </c>
+      <c r="C31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>5</v>
       </c>
+      <c r="C32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>6</v>
       </c>
+      <c r="C33">
+        <v>90</v>
+      </c>
+      <c r="D33">
+        <v>90</v>
+      </c>
+      <c r="E33">
+        <v>90</v>
+      </c>
+      <c r="F33">
+        <v>90</v>
+      </c>
+      <c r="G33">
+        <v>90</v>
+      </c>
+      <c r="H33">
+        <v>90</v>
+      </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="4"/>
-      <c r="M42" s="4"/>
-      <c r="N42" s="4"/>
-      <c r="O42" s="4"/>
-      <c r="P42" s="4"/>
-      <c r="Q42" s="4"/>
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
+      <c r="O42" s="3"/>
+      <c r="P42" s="3"/>
+      <c r="Q42" s="3"/>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
@@ -1066,10 +1438,10 @@
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="K45" s="1" t="s">
+      <c r="K45" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="L45" s="1"/>
+      <c r="L45" s="8"/>
       <c r="N45" t="s">
         <v>34</v>
       </c>
@@ -1112,7 +1484,7 @@
       <c r="B48" t="s">
         <v>20</v>
       </c>
-      <c r="K48" s="2" t="s">
+      <c r="K48" s="1" t="s">
         <v>31</v>
       </c>
       <c r="N48">
@@ -1140,7 +1512,7 @@
       <c r="B50" t="s">
         <v>22</v>
       </c>
-      <c r="K50" s="2" t="s">
+      <c r="K50" s="1" t="s">
         <v>30</v>
       </c>
       <c r="N50">
@@ -1162,15 +1534,15 @@
       </c>
     </row>
     <row r="53" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
@@ -1190,36 +1562,36 @@
       </c>
     </row>
     <row r="55" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
     </row>
     <row r="58" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="59" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
-      <c r="G59" s="4"/>
-      <c r="H59" s="4"/>
-      <c r="I59" s="4"/>
-      <c r="J59" s="4"/>
-      <c r="K59" s="4"/>
-      <c r="L59" s="4"/>
-      <c r="M59" s="4"/>
-      <c r="N59" s="4"/>
-      <c r="O59" s="4"/>
-      <c r="P59" s="4"/>
-      <c r="Q59" s="4"/>
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
+      <c r="L59" s="3"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="3"/>
+      <c r="O59" s="3"/>
+      <c r="P59" s="3"/>
+      <c r="Q59" s="3"/>
     </row>
     <row r="61" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
@@ -1280,7 +1652,7 @@
         <v>1.85</v>
       </c>
       <c r="K64">
-        <v>1.7</v>
+        <v>2.15</v>
       </c>
       <c r="M64" t="s">
         <v>46</v>
@@ -1314,7 +1686,7 @@
       <c r="Y65" t="s">
         <v>60</v>
       </c>
-      <c r="AA65" s="8" t="s">
+      <c r="AA65" s="7" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1338,7 +1710,7 @@
         <v>1.6</v>
       </c>
       <c r="K66">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="U66" t="s">
         <v>13</v>
@@ -1346,7 +1718,7 @@
       <c r="V66" t="s">
         <v>51</v>
       </c>
-      <c r="Y66" s="6" t="s">
+      <c r="Y66" s="5" t="s">
         <v>58</v>
       </c>
       <c r="AA66" t="s">
@@ -1360,7 +1732,7 @@
       <c r="V67" t="s">
         <v>54</v>
       </c>
-      <c r="Y67" s="7" t="s">
+      <c r="Y67" s="6" t="s">
         <v>59</v>
       </c>
       <c r="AA67">
@@ -1387,7 +1759,7 @@
         <v>1.85</v>
       </c>
       <c r="K68">
-        <v>1.6</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="U68" t="s">
         <v>15</v>
@@ -1395,10 +1767,10 @@
       <c r="V68" t="s">
         <v>56</v>
       </c>
-      <c r="Y68" s="5" t="s">
+      <c r="Y68" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AA68" s="2" t="s">
+      <c r="AA68" s="1" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1422,7 +1794,7 @@
         <v>1.4</v>
       </c>
       <c r="K70">
-        <v>1.7</v>
+        <v>2.2799999999999998</v>
       </c>
     </row>
     <row r="72" spans="1:27" x14ac:dyDescent="0.25">

</xml_diff>